<commit_message>
updated list of participants
</commit_message>
<xml_diff>
--- a/docs/participants_list_tdf2024.xlsx
+++ b/docs/participants_list_tdf2024.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11028"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10312"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/enrique.montes/Documents/p2p-tierradelfuego-workshop/docs/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/enriquemontes/p2p-tierradelfuego-workshop/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8C1D061-C8E0-714A-A8CB-A510A1423A24}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3577D02A-E6D3-2847-8ADF-102BA54D204F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="51200" windowHeight="27180" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="35840" windowHeight="20920" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="210" uniqueCount="115">
   <si>
     <t xml:space="preserve">Enrique </t>
   </si>
@@ -36,9 +36,6 @@
     <t>U. Miami CIMAS / NOAA AOML</t>
   </si>
   <si>
-    <t>USA</t>
-  </si>
-  <si>
     <t xml:space="preserve">Gregorio </t>
   </si>
   <si>
@@ -213,9 +210,6 @@
     <t>Massaccesi</t>
   </si>
   <si>
-    <t>APN Ushuaia</t>
-  </si>
-  <si>
     <t xml:space="preserve">Luciana </t>
   </si>
   <si>
@@ -334,13 +328,55 @@
   </si>
   <si>
     <t>Participante</t>
+  </si>
+  <si>
+    <t>Estados Unidos</t>
+  </si>
+  <si>
+    <t>Juan</t>
+  </si>
+  <si>
+    <t>Marcelo</t>
+  </si>
+  <si>
+    <t>Almirón</t>
+  </si>
+  <si>
+    <t>Alejandro</t>
+  </si>
+  <si>
+    <t>Lautaro</t>
+  </si>
+  <si>
+    <t>Martin</t>
+  </si>
+  <si>
+    <t>Natalia</t>
+  </si>
+  <si>
+    <t>Paulucci</t>
+  </si>
+  <si>
+    <t>Martinez</t>
+  </si>
+  <si>
+    <t>Laura</t>
+  </si>
+  <si>
+    <t>Wolinski</t>
+  </si>
+  <si>
+    <t>APN Parque Nacional Tierra del Fuego</t>
+  </si>
+  <si>
+    <t>Secretaría de Ambiente - Tierra del Fuego Recursos Hidricos</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -377,6 +413,13 @@
       <color rgb="FF000000"/>
       <name val="Aptos"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -398,7 +441,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -407,6 +450,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -622,13 +666,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:S999"/>
+  <dimension ref="A1:Q999"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="141" zoomScaleNormal="141" workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="M26" sqref="M26"/>
+      <selection pane="bottomRight" activeCell="C33" sqref="C33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -638,24 +682,24 @@
     <col min="3" max="3" width="51.83203125" customWidth="1"/>
     <col min="4" max="4" width="17.33203125" customWidth="1"/>
     <col min="5" max="5" width="34.5" customWidth="1"/>
-    <col min="6" max="19" width="10.6640625" customWidth="1"/>
+    <col min="6" max="17" width="10.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>95</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>97</v>
       </c>
       <c r="F1" s="1"/>
       <c r="G1" s="1"/>
@@ -669,10 +713,8 @@
       <c r="O1" s="1"/>
       <c r="P1" s="1"/>
       <c r="Q1" s="1"/>
-      <c r="R1" s="1"/>
-      <c r="S1" s="1"/>
-    </row>
-    <row r="2" spans="1:19" ht="16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="2" spans="1:17" ht="16" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
@@ -683,597 +725,696 @@
         <v>2</v>
       </c>
       <c r="D2" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" ht="16" x14ac:dyDescent="0.2">
+      <c r="A3" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="B3" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" ht="16" x14ac:dyDescent="0.2">
+      <c r="A4" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" ht="16" x14ac:dyDescent="0.2">
+      <c r="A5" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" ht="16" x14ac:dyDescent="0.2">
+      <c r="A6" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="E6" s="4" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="3" spans="1:19" ht="16" x14ac:dyDescent="0.2">
-      <c r="A3" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="4" spans="1:19" ht="16" x14ac:dyDescent="0.2">
-      <c r="A4" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C4" s="3" t="s">
+    <row r="7" spans="1:17" ht="16" x14ac:dyDescent="0.2">
+      <c r="A7" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" ht="16" x14ac:dyDescent="0.2">
+      <c r="A8" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17" ht="16" x14ac:dyDescent="0.2">
+      <c r="A9" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A10" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="D10" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="D4" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="E4" s="3" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="5" spans="1:19" ht="16" x14ac:dyDescent="0.2">
-      <c r="A5" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="E5" s="3" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="6" spans="1:19" ht="16" x14ac:dyDescent="0.2">
-      <c r="A6" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="D6" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="E6" s="4" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="7" spans="1:19" ht="16" x14ac:dyDescent="0.2">
-      <c r="A7" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="C7" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="D7" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="E7" s="3" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="8" spans="1:19" ht="16" x14ac:dyDescent="0.2">
-      <c r="A8" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="C8" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="D8" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="E8" s="3" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="9" spans="1:19" ht="16" x14ac:dyDescent="0.2">
-      <c r="A9" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="C9" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="D9" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="E9" s="3" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A10" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="B10" s="5" t="s">
+      <c r="E10" s="4" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A11" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="C11" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="C10" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="D10" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="E10" s="4" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A11" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="B11" s="5" t="s">
+      <c r="D11" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E11" s="4" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A12" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="C11" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="D11" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="E11" s="4" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A12" s="4" t="s">
+      <c r="B12" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="B12" s="4" t="s">
+      <c r="C12" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="C12" s="3" t="s">
+      <c r="D12" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E12" s="4" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17" ht="16" x14ac:dyDescent="0.2">
+      <c r="A13" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="D12" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="E12" s="4" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="13" spans="1:19" ht="16" x14ac:dyDescent="0.2">
-      <c r="A13" s="2" t="s">
+      <c r="B13" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="B13" s="2" t="s">
+      <c r="C13" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="D13" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E13" s="4" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="14" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A14" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="C13" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="D13" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="E13" s="4" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A14" s="4" t="s">
+      <c r="B14" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="B14" s="4" t="s">
+      <c r="C14" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="C14" s="3" t="s">
+      <c r="D14" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E14" s="4" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="15" spans="1:17" ht="16" x14ac:dyDescent="0.2">
+      <c r="A15" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="D14" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="E14" s="4" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="15" spans="1:19" ht="16" x14ac:dyDescent="0.2">
-      <c r="A15" s="2" t="s">
+      <c r="B15" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="B15" s="2" t="s">
+      <c r="C15" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="C15" s="2" t="s">
+      <c r="D15" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E15" s="4" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="16" spans="1:17" ht="16" x14ac:dyDescent="0.2">
+      <c r="A16" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="D15" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E15" s="4" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="16" spans="1:19" ht="16" x14ac:dyDescent="0.2">
-      <c r="A16" s="2" t="s">
+      <c r="B16" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="B16" s="2" t="s">
+      <c r="C16" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="C16" s="2" t="s">
-        <v>45</v>
-      </c>
       <c r="D16" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E16" s="4" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="17" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A17" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="B17" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="B17" s="2" t="s">
-        <v>47</v>
-      </c>
       <c r="C17" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E17" s="4" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="18" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A18" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="B18" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="B18" s="2" t="s">
-        <v>49</v>
-      </c>
       <c r="C18" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E18" s="4" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="19" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A19" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="B19" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="B19" s="2" t="s">
+      <c r="C19" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="C19" s="2" t="s">
-        <v>52</v>
-      </c>
       <c r="D19" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E19" s="4" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="20" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="B20" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="B20" s="2" t="s">
-        <v>54</v>
-      </c>
       <c r="C20" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E20" s="4" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="21" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="B21" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="B21" s="2" t="s">
+      <c r="C21" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="C21" s="2" t="s">
-        <v>57</v>
-      </c>
       <c r="D21" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E21" s="4" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="22" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="B22" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="B22" s="2" t="s">
-        <v>59</v>
-      </c>
       <c r="C22" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E22" s="4" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="23" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="B23" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="B23" s="2" t="s">
-        <v>61</v>
-      </c>
       <c r="C23" s="2" t="s">
-        <v>62</v>
+        <v>113</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E23" s="4" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="24" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="2" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>62</v>
+        <v>113</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E24" s="4" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="25" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="2" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>62</v>
+        <v>113</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E25" s="4" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="26" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="C26" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="B26" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="C26" s="2" t="s">
-        <v>69</v>
-      </c>
       <c r="D26" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E26" s="4" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="27" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="2" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E27" s="4" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="28" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="C28" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="B28" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="C28" s="2" t="s">
-        <v>74</v>
-      </c>
       <c r="D28" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E28" s="4" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="29" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="C29" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="B29" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="C29" s="2" t="s">
-        <v>77</v>
-      </c>
       <c r="D29" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E29" s="4" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="30" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="C30" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="B30" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="C30" s="2" t="s">
-        <v>80</v>
-      </c>
       <c r="D30" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E30" s="4" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="31" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="2" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E31" s="4" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="32" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="2" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E32" s="4" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="33" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="2" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>62</v>
+        <v>113</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E33" s="4" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="34" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="2" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D34" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E34" s="4" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="35" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="2" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="D35" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E35" s="4" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="36" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="2" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="D36" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E36" s="4" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A37" s="6" t="s">
+        <v>103</v>
+      </c>
+      <c r="B37" s="6" t="s">
+        <v>104</v>
+      </c>
+      <c r="C37" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="D37" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E37" s="4" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A38" s="6" t="s">
+        <v>105</v>
+      </c>
+      <c r="B38" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="C38" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="D38" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E38" s="4" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A39" s="6" t="s">
+        <v>106</v>
+      </c>
+      <c r="B39" s="6" t="s">
+        <v>107</v>
+      </c>
+      <c r="C39" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="D39" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E39" s="4" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A40" s="6" t="s">
+        <v>108</v>
+      </c>
+      <c r="B40" s="6" t="s">
+        <v>109</v>
+      </c>
+      <c r="C40" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="D40" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E40" s="4" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A41" s="6" t="s">
         <v>102</v>
       </c>
-    </row>
-    <row r="37" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="38" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="39" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="40" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="41" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="42" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="43" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+      <c r="B41" s="6" t="s">
+        <v>110</v>
+      </c>
+      <c r="C41" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="D41" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E41" s="4" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A42" s="6" t="s">
+        <v>111</v>
+      </c>
+      <c r="B42" s="6" t="s">
+        <v>112</v>
+      </c>
+      <c r="C42" s="6" t="s">
+        <v>114</v>
+      </c>
+      <c r="D42" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E42" s="4" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A43" s="6"/>
+      <c r="B43" s="6"/>
+    </row>
     <row r="44" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="45" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="46" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>

</xml_diff>